<commit_message>
add auto evalution pipeline
</commit_message>
<xml_diff>
--- a/evaluation_dataset/query.xlsx
+++ b/evaluation_dataset/query.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuyifan/Desktop/agent/Pipeline/evaluation_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F263084-9DF1-9C49-9D15-E94E6940AE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE652FB-05BB-D945-A971-268784C908EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="2680" windowWidth="28240" windowHeight="17440" xr2:uid="{502EEE7A-63F9-274F-B3D6-1302183ED8D1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD05CB4C-965B-7549-915C-B0D561C52619}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -474,6 +474,61 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>12306</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>12306</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>12306</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>12306</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>12306</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>